<commit_message>
21.08.19 today Sales Details
</commit_message>
<xml_diff>
--- a/August/Others/Price List Update_10.08.2018.xlsx
+++ b/August/Others/Price List Update_10.08.2018.xlsx
@@ -345,7 +345,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> Symphony Price List                           Date:18.08.19</t>
+    <t xml:space="preserve"> Symphony Price List                           Date:21.08.19</t>
   </si>
 </sst>
 </file>
@@ -976,8 +976,8 @@
   </sheetPr>
   <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>

</xml_diff>